<commit_message>
fixing trash files for pinouts and board
</commit_message>
<xml_diff>
--- a/rfm69/rfm69_32u4/rev-/docs/Pinouts.xlsx
+++ b/rfm69/rfm69_32u4/rev-/docs/Pinouts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Feather" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="159">
   <si>
     <t xml:space="preserve">HEADER</t>
   </si>
@@ -368,6 +368,126 @@
     <t xml:space="preserve">To Device Pin</t>
   </si>
   <si>
+    <t xml:space="preserve">12_RF_CS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eagle Trace Signal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VCC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+3V3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.3Vreg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uC Power</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VCC1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UVCC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AVCC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AVCC1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UCAP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XTAL1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMD Resonator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 MHz Crystal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XTAL2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UGND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GROUND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GND1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GND2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GND3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7_RELAY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RELAY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relay digital Control Pin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digital Pin 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9_SD_CD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SD Card</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4_SD_CS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2_RF_DIO0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15 (SCK)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digital Pin 15 (SCK)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15_SCK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF, SD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16 (MOSI)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16_MOSI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14 (MISO)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14_MISO</t>
+  </si>
+  <si>
     <t xml:space="preserve">0_RX</t>
   </si>
   <si>
@@ -378,36 +498,6 @@
   </si>
   <si>
     <t xml:space="preserve">1_GPS_RXD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12_RF_CS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NSS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RELAY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Relay digital Control Pin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4_SD_CS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7_SD_CD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7_RELAY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Digital Pin 9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9_SD_CD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SD Card</t>
   </si>
 </sst>
 </file>
@@ -551,9 +641,9 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.96356275303644"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.4615384615385"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="16.1740890688259"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="34.8137651821862"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="35.0283400809717"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1258,19 +1348,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:G37"/>
+  <dimension ref="A2:G51"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E38" activeCellId="0" sqref="E38"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.1174089068826"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.47773279352227"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="16.1740890688259"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="34.8137651821862"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.4251012145749"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="35.0283400809717"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1297,655 +1387,896 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="n">
-        <v>13</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="n">
-        <v>14</v>
-      </c>
+      <c r="A4" s="2"/>
       <c r="B4" s="0" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>15</v>
+        <v>21</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>22</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2"/>
+      <c r="A6" s="2" t="n">
+        <v>37</v>
+      </c>
       <c r="B6" s="0" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>18</v>
+        <v>25</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="E7" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="0" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="n">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>22</v>
+        <v>30</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="n">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>22</v>
+        <v>35</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="n">
+        <v>41</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>30</v>
+      <c r="E10" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>40</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="n">
-        <v>40</v>
-      </c>
+      <c r="A11" s="2"/>
       <c r="B11" s="0" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="n">
-        <v>41</v>
-      </c>
+      <c r="A12" s="2"/>
       <c r="B12" s="0" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="n">
-        <v>9</v>
-      </c>
+      <c r="A13" s="2"/>
       <c r="B13" s="0" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="E13" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="F13" s="0" t="s">
+        <v>62</v>
+      </c>
       <c r="G13" s="0" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2"/>
       <c r="B14" s="0" t="s">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="E14" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="F14" s="0" t="s">
+        <v>66</v>
+      </c>
       <c r="G14" s="0" t="s">
-        <v>47</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2"/>
-      <c r="B15" s="0" t="s">
-        <v>48</v>
+      <c r="B15" s="2" t="n">
+        <v>13</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>10</v>
+        <v>72</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>73</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="n">
-        <v>20</v>
-      </c>
-      <c r="B16" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="C16" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="D16" s="0" t="s">
+      <c r="E16" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="E16" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="F16" s="0" t="s">
-        <v>54</v>
-      </c>
       <c r="G16" s="0" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="n">
-        <v>21</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>117</v>
+        <v>12</v>
+      </c>
+      <c r="B17" s="2" t="n">
+        <v>11</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>56</v>
+        <v>79</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>118</v>
+        <v>80</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="G17" s="0" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2"/>
-      <c r="B18" s="0" t="s">
-        <v>17</v>
+      <c r="B18" s="2" t="n">
+        <v>10</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>18</v>
+        <v>82</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>17</v>
+        <v>83</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="G18" s="0" t="s">
-        <v>18</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2"/>
-      <c r="B19" s="0" t="s">
-        <v>59</v>
+      <c r="B19" s="2" t="n">
+        <v>6</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>60</v>
+        <v>89</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>61</v>
+        <v>90</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="G19" s="0" t="s">
-        <v>60</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2"/>
-      <c r="B20" s="0" t="s">
-        <v>62</v>
+      <c r="B20" s="2" t="n">
+        <v>5</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>63</v>
+        <v>92</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>64</v>
+        <v>93</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="G20" s="0" t="s">
-        <v>65</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2"/>
-      <c r="B21" s="0" t="s">
-        <v>66</v>
+      <c r="A21" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="B21" s="2" t="n">
+        <v>3</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>67</v>
+        <v>95</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>68</v>
+        <v>96</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>66</v>
+        <v>97</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>69</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2"/>
+      <c r="A22" s="2" t="n">
+        <v>28</v>
+      </c>
       <c r="B22" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="C22" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="F22" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="G22" s="0" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="2" t="n">
-        <v>26</v>
-      </c>
-      <c r="B23" s="2" t="n">
-        <v>12</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="F23" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="G23" s="0" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="2" t="n">
-        <v>12</v>
-      </c>
-      <c r="B24" s="2" t="n">
+      <c r="B25" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" s="0" t="s">
         <v>11</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="E24" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="F24" s="0" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="C25" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="D25" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="E25" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="F25" s="0" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="n">
-        <v>29</v>
-      </c>
-      <c r="B26" s="5" t="n">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>85</v>
+        <v>118</v>
       </c>
       <c r="D26" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="G26" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="E26" s="0" t="s">
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="2" t="n">
+        <v>34</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="G27" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="F26" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="G26" s="0" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2" t="n">
-        <v>6</v>
-      </c>
-      <c r="C27" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="D27" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="E27" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="F27" s="0" t="s">
-        <v>91</v>
-      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2" t="n">
-        <v>5</v>
+      <c r="A28" s="2" t="n">
+        <v>2</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>92</v>
+        <v>123</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>93</v>
+        <v>124</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>35</v>
+        <v>125</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>94</v>
+        <v>125</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="n">
-        <v>18</v>
-      </c>
-      <c r="B29" s="2" t="n">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>95</v>
+        <v>126</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>96</v>
+        <v>119</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>22</v>
+        <v>120</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>97</v>
+        <v>119</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>98</v>
+        <v>121</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="n">
-        <v>19</v>
-      </c>
-      <c r="B30" s="2" t="n">
-        <v>2</v>
+        <v>44</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>99</v>
+        <v>127</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>100</v>
+        <v>119</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>35</v>
+        <v>120</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2" t="n">
-        <v>4</v>
+      <c r="A31" s="2" t="n">
+        <v>42</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>103</v>
+        <v>15</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>123</v>
+        <v>119</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="F31" s="0" t="s">
+        <v>119</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>105</v>
+        <v>16</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B32" s="2" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>106</v>
+        <v>128</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="G32" s="0" t="s">
-        <v>108</v>
+        <v>119</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="F32" s="0" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="n">
-        <v>28</v>
-      </c>
-      <c r="B33" s="2" t="n">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>109</v>
+        <v>129</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>110</v>
+        <v>129</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="F33" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>111</v>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="F34" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="G34" s="0" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="G35" s="0" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B36" s="2" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>106</v>
+        <v>17</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>125</v>
+        <v>17</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>121</v>
+        <v>17</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="G37" s="0" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="2" t="n">
+        <v>35</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="F38" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="G38" s="0" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="2" t="n">
+        <v>43</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="G39" s="0" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="2"/>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="2"/>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="2"/>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B43" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="F43" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="G43" s="0" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="2" t="n">
         <v>29</v>
       </c>
-      <c r="B37" s="5" t="n">
+      <c r="B44" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="C37" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="D37" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="E37" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="F37" s="2" t="s">
+      <c r="C44" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="E44" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="F44" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="G37" s="0" t="s">
+      <c r="G44" s="0" t="s">
         <v>108</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="B45" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="G45" s="0" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="B46" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="E46" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="F46" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="G46" s="0" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="E47" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="G47" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="E48" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="G48" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="E49" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="G49" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="D50" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="E50" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F50" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="G50" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="E51" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F51" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="G51" s="0" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>